<commit_message>
Alterações na tabela de comparação RVND x ILS
</commit_message>
<xml_diff>
--- a/Arquivos/Comparações/RVND x ILS.xlsx
+++ b/Arquivos/Comparações/RVND x ILS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="75">
   <si>
     <t>Comparação ILS e RVND com k = n/4</t>
   </si>
@@ -1264,8 +1264,8 @@
   <sheetPr/>
   <dimension ref="B3:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="N10" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -2020,9 +2020,8 @@
       <c r="E18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Iguais</v>
+      <c r="F18" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>22</v>
@@ -4479,7 +4478,7 @@
       </c>
       <c r="D71" s="14">
         <f>COUNTIF(F5:F66,"Iguais")+COUNTIF(M5:M66,"Iguais")+COUNTIF(T5:T66,"Iguais")</f>
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementação de nova forma de pertubarção
</commit_message>
<xml_diff>
--- a/Arquivos/Comparações/RVND x ILS.xlsx
+++ b/Arquivos/Comparações/RVND x ILS.xlsx
@@ -246,10 +246,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="0_ "/>
   </numFmts>
   <fonts count="22">
@@ -275,8 +275,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -291,34 +312,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -328,15 +321,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -350,8 +335,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,9 +359,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,10 +391,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -396,17 +405,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -428,72 +428,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -506,13 +440,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,43 +500,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,13 +518,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,19 +602,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,39 +650,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -694,6 +661,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,11 +691,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -747,157 +736,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -917,12 +917,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1264,8 +1258,8 @@
   <sheetPr/>
   <dimension ref="B3:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -1326,34 +1320,34 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="Q4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="S4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="T4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1380,7 +1374,7 @@
       <c r="J5" s="5">
         <v>140</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="9">
         <v>1286.16</v>
       </c>
       <c r="L5" s="6">
@@ -1393,13 +1387,13 @@
       <c r="P5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="1">
         <v>210</v>
       </c>
-      <c r="R5" s="11">
+      <c r="R5" s="9">
         <v>1925.22</v>
       </c>
-      <c r="S5" s="12">
+      <c r="S5" s="10">
         <v>1902.27</v>
       </c>
       <c r="T5" s="7" t="str">
@@ -1430,7 +1424,7 @@
       <c r="J6" s="5">
         <v>24</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="9">
         <v>3231</v>
       </c>
       <c r="L6" s="6">
@@ -1443,13 +1437,13 @@
       <c r="P6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="Q6" s="1">
         <v>36</v>
       </c>
-      <c r="R6" s="11">
+      <c r="R6" s="9">
         <v>6348</v>
       </c>
-      <c r="S6" s="12">
+      <c r="S6" s="10">
         <v>6252</v>
       </c>
       <c r="T6" s="7" t="str">
@@ -1480,7 +1474,7 @@
       <c r="J7" s="5">
         <v>266</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="9">
         <v>11954</v>
       </c>
       <c r="L7" s="6">
@@ -1493,10 +1487,10 @@
       <c r="P7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="Q7" s="1">
         <v>399</v>
       </c>
-      <c r="R7" s="11">
+      <c r="R7" s="9">
         <v>18238</v>
       </c>
       <c r="S7" s="6" t="s">
@@ -1530,7 +1524,7 @@
       <c r="J8" s="5">
         <v>14</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="9">
         <v>581</v>
       </c>
       <c r="L8" s="6">
@@ -1543,13 +1537,13 @@
       <c r="P8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="8">
+      <c r="Q8" s="1">
         <v>21</v>
       </c>
-      <c r="R8" s="11">
+      <c r="R8" s="9">
         <v>1035</v>
       </c>
-      <c r="S8" s="12">
+      <c r="S8" s="10">
         <v>1040</v>
       </c>
       <c r="T8" s="7" t="str">
@@ -1580,7 +1574,7 @@
       <c r="J9" s="5">
         <v>14</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="9">
         <v>692</v>
       </c>
       <c r="L9" s="6">
@@ -1593,13 +1587,13 @@
       <c r="P9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="Q9" s="1">
         <v>21</v>
       </c>
-      <c r="R9" s="11">
+      <c r="R9" s="9">
         <v>1128</v>
       </c>
-      <c r="S9" s="12">
+      <c r="S9" s="10">
         <v>1159</v>
       </c>
       <c r="T9" s="7" t="str">
@@ -1630,7 +1624,7 @@
       <c r="J10" s="5">
         <v>26</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="9">
         <v>1766.5</v>
       </c>
       <c r="L10" s="6">
@@ -1643,13 +1637,13 @@
       <c r="P10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="Q10" s="1">
         <v>39</v>
       </c>
-      <c r="R10" s="11">
+      <c r="R10" s="9">
         <v>3910.64</v>
       </c>
-      <c r="S10" s="12">
+      <c r="S10" s="10">
         <v>3910.64</v>
       </c>
       <c r="T10" s="7" t="str">
@@ -1680,7 +1674,7 @@
       <c r="J11" s="5">
         <v>63</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="9">
         <v>27397.27</v>
       </c>
       <c r="L11" s="6">
@@ -1693,13 +1687,13 @@
       <c r="P11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="8">
+      <c r="Q11" s="1">
         <v>95</v>
       </c>
-      <c r="R11" s="11">
+      <c r="R11" s="9">
         <v>49142.24</v>
       </c>
-      <c r="S11" s="12">
+      <c r="S11" s="10">
         <v>50282.14</v>
       </c>
       <c r="T11" s="7" t="str">
@@ -1730,7 +1724,7 @@
       <c r="J12" s="5">
         <v>29</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="9">
         <v>6805</v>
       </c>
       <c r="L12" s="6">
@@ -1743,13 +1737,13 @@
       <c r="P12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="8">
+      <c r="Q12" s="1">
         <v>43</v>
       </c>
-      <c r="R12" s="11">
+      <c r="R12" s="9">
         <v>10285</v>
       </c>
-      <c r="S12" s="12">
+      <c r="S12" s="10">
         <v>10035</v>
       </c>
       <c r="T12" s="7" t="str">
@@ -1780,7 +1774,7 @@
       <c r="J13" s="5">
         <v>90</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="9">
         <v>950</v>
       </c>
       <c r="L13" s="6">
@@ -1793,13 +1787,13 @@
       <c r="P13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q13" s="8">
+      <c r="Q13" s="1">
         <v>135</v>
       </c>
-      <c r="R13" s="11">
+      <c r="R13" s="9">
         <v>1460</v>
       </c>
-      <c r="S13" s="12">
+      <c r="S13" s="10">
         <v>1460</v>
       </c>
       <c r="T13" s="7" t="str">
@@ -1830,7 +1824,7 @@
       <c r="J14" s="5">
         <v>7</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="9">
         <v>1140.19</v>
       </c>
       <c r="L14" s="6">
@@ -1843,13 +1837,13 @@
       <c r="P14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="Q14" s="8">
+      <c r="Q14" s="1">
         <v>10</v>
       </c>
-      <c r="R14" s="11">
+      <c r="R14" s="9">
         <v>1637.31</v>
       </c>
-      <c r="S14" s="12">
+      <c r="S14" s="10">
         <v>1637.31</v>
       </c>
       <c r="T14" s="7" t="str">
@@ -1880,7 +1874,7 @@
       <c r="J15" s="5">
         <v>65</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="9">
         <v>2541.67</v>
       </c>
       <c r="L15" s="6">
@@ -1893,13 +1887,13 @@
       <c r="P15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="8">
+      <c r="Q15" s="1">
         <v>97</v>
       </c>
-      <c r="R15" s="11">
+      <c r="R15" s="9">
         <v>3908.11</v>
       </c>
-      <c r="S15" s="12">
+      <c r="S15" s="10">
         <v>3884.41</v>
       </c>
       <c r="T15" s="7" t="str">
@@ -1930,7 +1924,7 @@
       <c r="J16" s="5">
         <v>75</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="9">
         <v>2907.65</v>
       </c>
       <c r="L16" s="6">
@@ -1943,13 +1937,13 @@
       <c r="P16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" s="8">
+      <c r="Q16" s="1">
         <v>112</v>
       </c>
-      <c r="R16" s="11">
+      <c r="R16" s="9">
         <v>4684.6</v>
       </c>
-      <c r="S16" s="12">
+      <c r="S16" s="10">
         <v>4599.97</v>
       </c>
       <c r="T16" s="7" t="str">
@@ -1980,7 +1974,7 @@
       <c r="J17" s="5">
         <v>21</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="9">
         <v>239</v>
       </c>
       <c r="L17" s="6">
@@ -1993,13 +1987,13 @@
       <c r="P17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Q17" s="8">
+      <c r="Q17" s="1">
         <v>31</v>
       </c>
-      <c r="R17" s="11">
+      <c r="R17" s="9">
         <v>401</v>
       </c>
-      <c r="S17" s="12">
+      <c r="S17" s="10">
         <v>401</v>
       </c>
       <c r="T17" s="7" t="str">
@@ -2029,7 +2023,7 @@
       <c r="J18" s="5">
         <v>25</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="9">
         <v>168.63</v>
       </c>
       <c r="L18" s="6">
@@ -2042,13 +2036,13 @@
       <c r="P18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q18" s="8">
+      <c r="Q18" s="1">
         <v>38</v>
       </c>
-      <c r="R18" s="11">
+      <c r="R18" s="9">
         <v>281.61</v>
       </c>
-      <c r="S18" s="12">
+      <c r="S18" s="10">
         <v>281.61</v>
       </c>
       <c r="T18" s="7" t="str">
@@ -2079,7 +2073,7 @@
       <c r="J19" s="5">
         <v>38</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K19" s="9">
         <v>221.22</v>
       </c>
       <c r="L19" s="6">
@@ -2092,13 +2086,13 @@
       <c r="P19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Q19" s="8">
+      <c r="Q19" s="1">
         <v>57</v>
       </c>
-      <c r="R19" s="11">
+      <c r="R19" s="9">
         <v>340.02</v>
       </c>
-      <c r="S19" s="12">
+      <c r="S19" s="10">
         <v>340.02</v>
       </c>
       <c r="T19" s="7" t="str">
@@ -2129,7 +2123,7 @@
       <c r="J20" s="5">
         <v>50</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="9">
         <v>286.97</v>
       </c>
       <c r="L20" s="6">
@@ -2142,13 +2136,13 @@
       <c r="P20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q20" s="8">
+      <c r="Q20" s="1">
         <v>75</v>
       </c>
-      <c r="R20" s="11">
+      <c r="R20" s="9">
         <v>438.75</v>
       </c>
-      <c r="S20" s="12">
+      <c r="S20" s="10">
         <v>438.75</v>
       </c>
       <c r="T20" s="7" t="str">
@@ -2179,7 +2173,7 @@
       <c r="J21" s="5">
         <v>13</v>
       </c>
-      <c r="K21" s="11">
+      <c r="K21" s="9">
         <v>317</v>
       </c>
       <c r="L21" s="6">
@@ -2192,13 +2186,13 @@
       <c r="P21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Q21" s="8">
+      <c r="Q21" s="1">
         <v>19</v>
       </c>
-      <c r="R21" s="11">
+      <c r="R21" s="9">
         <v>599</v>
       </c>
-      <c r="S21" s="12">
+      <c r="S21" s="10">
         <v>559</v>
       </c>
       <c r="T21" s="7" t="str">
@@ -2229,7 +2223,7 @@
       <c r="J22" s="5">
         <v>131</v>
       </c>
-      <c r="K22" s="11">
+      <c r="K22" s="9">
         <v>1100.26</v>
       </c>
       <c r="L22" s="6">
@@ -2242,13 +2236,13 @@
       <c r="P22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q22" s="8">
+      <c r="Q22" s="1">
         <v>196</v>
       </c>
-      <c r="R22" s="11">
+      <c r="R22" s="9">
         <v>1640.39</v>
       </c>
-      <c r="S22" s="12">
+      <c r="S22" s="10">
         <v>1644.53</v>
       </c>
       <c r="T22" s="7" t="str">
@@ -2279,7 +2273,7 @@
       <c r="J23" s="5">
         <v>8</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="9">
         <v>359</v>
       </c>
       <c r="L23" s="6">
@@ -2292,13 +2286,13 @@
       <c r="P23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q23" s="8">
+      <c r="Q23" s="1">
         <v>12</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R23" s="9">
         <v>640</v>
       </c>
-      <c r="S23" s="12">
+      <c r="S23" s="10">
         <v>640</v>
       </c>
       <c r="T23" s="7" t="str">
@@ -2329,7 +2323,7 @@
       <c r="J24" s="5">
         <v>10</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="9">
         <v>711</v>
       </c>
       <c r="L24" s="6">
@@ -2342,13 +2336,13 @@
       <c r="P24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Q24" s="8">
+      <c r="Q24" s="1">
         <v>15</v>
       </c>
-      <c r="R24" s="11">
+      <c r="R24" s="9">
         <v>1331</v>
       </c>
-      <c r="S24" s="12">
+      <c r="S24" s="10">
         <v>1331</v>
       </c>
       <c r="T24" s="7" t="str">
@@ -2379,7 +2373,7 @@
       <c r="J25" s="5">
         <v>12</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="9">
         <v>413</v>
       </c>
       <c r="L25" s="6">
@@ -2392,13 +2386,13 @@
       <c r="P25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q25" s="8">
+      <c r="Q25" s="1">
         <v>18</v>
       </c>
-      <c r="R25" s="11">
+      <c r="R25" s="9">
         <v>794</v>
       </c>
-      <c r="S25" s="12">
+      <c r="S25" s="10">
         <v>794</v>
       </c>
       <c r="T25" s="7" t="str">
@@ -2429,7 +2423,7 @@
       <c r="J26" s="5">
         <v>24</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K26" s="9">
         <v>1705</v>
       </c>
       <c r="L26" s="6">
@@ -2442,13 +2436,13 @@
       <c r="P26" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Q26" s="8">
+      <c r="Q26" s="1">
         <v>36</v>
       </c>
-      <c r="R26" s="11">
+      <c r="R26" s="9">
         <v>3054</v>
       </c>
-      <c r="S26" s="12">
+      <c r="S26" s="10">
         <v>3054</v>
       </c>
       <c r="T26" s="7" t="str">
@@ -2479,7 +2473,7 @@
       <c r="J27" s="5">
         <v>48</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="9">
         <v>20435.51</v>
       </c>
       <c r="L27" s="6">
@@ -2492,13 +2486,13 @@
       <c r="P27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q27" s="8">
+      <c r="Q27" s="1">
         <v>72</v>
       </c>
-      <c r="R27" s="11">
+      <c r="R27" s="9">
         <v>36699.98</v>
       </c>
-      <c r="S27" s="12">
+      <c r="S27" s="10">
         <v>36699.98</v>
       </c>
       <c r="T27" s="7" t="str">
@@ -2529,7 +2523,7 @@
       <c r="J28" s="5">
         <v>60</v>
       </c>
-      <c r="K28" s="11">
+      <c r="K28" s="9">
         <v>3091</v>
       </c>
       <c r="L28" s="6">
@@ -2542,13 +2536,13 @@
       <c r="P28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q28" s="8">
+      <c r="Q28" s="1">
         <v>90</v>
       </c>
-      <c r="R28" s="11">
+      <c r="R28" s="9">
         <v>4537</v>
       </c>
-      <c r="S28" s="12">
+      <c r="S28" s="10">
         <v>4542</v>
       </c>
       <c r="T28" s="7" t="str">
@@ -2579,7 +2573,7 @@
       <c r="J29" s="5">
         <v>24</v>
       </c>
-      <c r="K29" s="11">
+      <c r="K29" s="9">
         <v>5511</v>
       </c>
       <c r="L29" s="6">
@@ -2592,13 +2586,13 @@
       <c r="P29" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q29" s="8">
+      <c r="Q29" s="1">
         <v>36</v>
       </c>
-      <c r="R29" s="11">
+      <c r="R29" s="9">
         <v>7612</v>
       </c>
-      <c r="S29" s="12">
+      <c r="S29" s="10">
         <v>7650</v>
       </c>
       <c r="T29" s="7" t="str">
@@ -2629,7 +2623,7 @@
       <c r="J30" s="5">
         <v>50</v>
       </c>
-      <c r="K30" s="11">
+      <c r="K30" s="9">
         <v>10075.59</v>
       </c>
       <c r="L30" s="6">
@@ -2642,13 +2636,13 @@
       <c r="P30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Q30" s="8">
+      <c r="Q30" s="1">
         <v>75</v>
       </c>
-      <c r="R30" s="11">
+      <c r="R30" s="9">
         <v>14544.38</v>
       </c>
-      <c r="S30" s="12">
+      <c r="S30" s="10">
         <v>14896.93</v>
       </c>
       <c r="T30" s="7" t="str">
@@ -2679,7 +2673,7 @@
       <c r="J31" s="5">
         <v>75</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K31" s="9">
         <v>14013.34</v>
       </c>
       <c r="L31" s="6">
@@ -2692,13 +2686,13 @@
       <c r="P31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q31" s="8">
+      <c r="Q31" s="1">
         <v>112</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R31" s="9">
         <v>19944.47</v>
       </c>
-      <c r="S31" s="12">
+      <c r="S31" s="10">
         <v>19154.06</v>
       </c>
       <c r="T31" s="7" t="str">
@@ -2729,7 +2723,7 @@
       <c r="J32" s="5">
         <v>100</v>
       </c>
-      <c r="K32" s="11">
+      <c r="K32" s="9">
         <v>12922.46</v>
       </c>
       <c r="L32" s="6">
@@ -2742,13 +2736,13 @@
       <c r="P32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q32" s="8">
+      <c r="Q32" s="1">
         <v>150</v>
       </c>
-      <c r="R32" s="11">
+      <c r="R32" s="9">
         <v>20463.14</v>
       </c>
-      <c r="S32" s="12">
+      <c r="S32" s="10">
         <v>20456.35</v>
       </c>
       <c r="T32" s="7" t="str">
@@ -2779,7 +2773,7 @@
       <c r="J33" s="5">
         <v>50</v>
       </c>
-      <c r="K33" s="11">
+      <c r="K33" s="9">
         <v>10708.33</v>
       </c>
       <c r="L33" s="6">
@@ -2792,13 +2786,13 @@
       <c r="P33" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Q33" s="8">
+      <c r="Q33" s="1">
         <v>75</v>
       </c>
-      <c r="R33" s="11">
+      <c r="R33" s="9">
         <v>15454.66</v>
       </c>
-      <c r="S33" s="12">
+      <c r="S33" s="10">
         <v>15454.66</v>
       </c>
       <c r="T33" s="7" t="str">
@@ -2829,7 +2823,7 @@
       <c r="J34" s="5">
         <v>75</v>
       </c>
-      <c r="K34" s="11">
+      <c r="K34" s="9">
         <v>11076.35</v>
       </c>
       <c r="L34" s="6">
@@ -2842,13 +2836,13 @@
       <c r="P34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q34" s="8">
+      <c r="Q34" s="1">
         <v>112</v>
       </c>
-      <c r="R34" s="11">
+      <c r="R34" s="9">
         <v>16688.08</v>
       </c>
-      <c r="S34" s="12">
+      <c r="S34" s="10">
         <v>16728.79</v>
       </c>
       <c r="T34" s="7" t="str">
@@ -2879,7 +2873,7 @@
       <c r="J35" s="5">
         <v>100</v>
       </c>
-      <c r="K35" s="11">
+      <c r="K35" s="9">
         <v>14033.62</v>
       </c>
       <c r="L35" s="6">
@@ -2892,13 +2886,13 @@
       <c r="P35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q35" s="8">
+      <c r="Q35" s="1">
         <v>150</v>
       </c>
-      <c r="R35" s="11">
+      <c r="R35" s="9">
         <v>20173.58</v>
       </c>
-      <c r="S35" s="12">
+      <c r="S35" s="10">
         <v>20134.61</v>
       </c>
       <c r="T35" s="7" t="str">
@@ -2929,7 +2923,7 @@
       <c r="J36" s="5">
         <v>50</v>
       </c>
-      <c r="K36" s="11">
+      <c r="K36" s="9">
         <v>8632.68</v>
       </c>
       <c r="L36" s="6">
@@ -2942,13 +2936,13 @@
       <c r="P36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q36" s="8">
+      <c r="Q36" s="1">
         <v>75</v>
       </c>
-      <c r="R36" s="11">
+      <c r="R36" s="9">
         <v>13951.85</v>
       </c>
-      <c r="S36" s="12">
+      <c r="S36" s="10">
         <v>13951.85</v>
       </c>
       <c r="T36" s="7" t="str">
@@ -2979,7 +2973,7 @@
       <c r="J37" s="5">
         <v>50</v>
       </c>
-      <c r="K37" s="11">
+      <c r="K37" s="9">
         <v>10204.13</v>
       </c>
       <c r="L37" s="6">
@@ -2992,13 +2986,13 @@
       <c r="P37" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q37" s="8">
+      <c r="Q37" s="1">
         <v>75</v>
       </c>
-      <c r="R37" s="11">
+      <c r="R37" s="9">
         <v>14779.43</v>
       </c>
-      <c r="S37" s="12">
+      <c r="S37" s="10">
         <v>14779.43</v>
       </c>
       <c r="T37" s="7" t="str">
@@ -3029,7 +3023,7 @@
       <c r="J38" s="5">
         <v>50</v>
       </c>
-      <c r="K38" s="11">
+      <c r="K38" s="9">
         <v>9060.14</v>
       </c>
       <c r="L38" s="6">
@@ -3042,13 +3036,13 @@
       <c r="P38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Q38" s="8">
+      <c r="Q38" s="1">
         <v>75</v>
       </c>
-      <c r="R38" s="11">
+      <c r="R38" s="9">
         <v>14943.31</v>
       </c>
-      <c r="S38" s="12">
+      <c r="S38" s="10">
         <v>14943.31</v>
       </c>
       <c r="T38" s="7" t="str">
@@ -3079,7 +3073,7 @@
       <c r="J39" s="5">
         <v>52</v>
       </c>
-      <c r="K39" s="11">
+      <c r="K39" s="9">
         <v>5425.48</v>
       </c>
       <c r="L39" s="6">
@@ -3092,13 +3086,13 @@
       <c r="P39" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q39" s="8">
+      <c r="Q39" s="1">
         <v>78</v>
       </c>
-      <c r="R39" s="11">
+      <c r="R39" s="9">
         <v>8397.36</v>
       </c>
-      <c r="S39" s="12">
+      <c r="S39" s="10">
         <v>8397.36</v>
       </c>
       <c r="T39" s="7" t="str">
@@ -3129,7 +3123,7 @@
       <c r="J40" s="5">
         <v>159</v>
       </c>
-      <c r="K40" s="11">
+      <c r="K40" s="9">
         <v>18685.55</v>
       </c>
       <c r="L40" s="6">
@@ -3142,13 +3136,13 @@
       <c r="P40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q40" s="8">
+      <c r="Q40" s="1">
         <v>238</v>
       </c>
-      <c r="R40" s="11">
+      <c r="R40" s="9">
         <v>28655.37</v>
       </c>
-      <c r="S40" s="12">
+      <c r="S40" s="10">
         <v>29009.41</v>
       </c>
       <c r="T40" s="7" t="str">
@@ -3179,7 +3173,7 @@
       <c r="J41" s="5">
         <v>689</v>
       </c>
-      <c r="K41" s="11">
+      <c r="K41" s="9">
         <v>26839.14</v>
       </c>
       <c r="L41" s="6">
@@ -3192,10 +3186,10 @@
       <c r="P41" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q41" s="8">
+      <c r="Q41" s="1">
         <v>1034</v>
       </c>
-      <c r="R41" s="11">
+      <c r="R41" s="9">
         <v>42522.62</v>
       </c>
       <c r="S41" s="6" t="s">
@@ -3228,7 +3222,7 @@
       <c r="J42" s="5">
         <v>280</v>
       </c>
-      <c r="K42" s="11">
+      <c r="K42" s="9">
         <v>1236</v>
       </c>
       <c r="L42" s="6">
@@ -3241,10 +3235,10 @@
       <c r="P42" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q42" s="8">
+      <c r="Q42" s="1">
         <v>420</v>
       </c>
-      <c r="R42" s="11">
+      <c r="R42" s="9">
         <v>2028</v>
       </c>
       <c r="S42" s="6" t="s">
@@ -3277,7 +3271,7 @@
       <c r="J43" s="5">
         <v>38</v>
       </c>
-      <c r="K43" s="11">
+      <c r="K43" s="9">
         <v>42006.67</v>
       </c>
       <c r="L43" s="6">
@@ -3290,13 +3284,13 @@
       <c r="P43" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Q43" s="8">
+      <c r="Q43" s="1">
         <v>57</v>
       </c>
-      <c r="R43" s="11">
+      <c r="R43" s="9">
         <v>61124.81</v>
       </c>
-      <c r="S43" s="12">
+      <c r="S43" s="10">
         <v>61124.81</v>
       </c>
       <c r="T43" s="7" t="str">
@@ -3327,7 +3321,7 @@
       <c r="J44" s="5">
         <v>52</v>
       </c>
-      <c r="K44" s="11">
+      <c r="K44" s="9">
         <v>15092.28</v>
       </c>
       <c r="L44" s="6">
@@ -3340,13 +3334,13 @@
       <c r="P44" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Q44" s="8">
+      <c r="Q44" s="1">
         <v>80</v>
       </c>
-      <c r="R44" s="11">
+      <c r="R44" s="9">
         <v>30429.58</v>
       </c>
-      <c r="S44" s="12">
+      <c r="S44" s="10">
         <v>30115.85</v>
       </c>
       <c r="T44" s="7" t="str">
@@ -3377,7 +3371,7 @@
       <c r="J45" s="5">
         <v>62</v>
       </c>
-      <c r="K45" s="11">
+      <c r="K45" s="9">
         <v>22935.61</v>
       </c>
       <c r="L45" s="6">
@@ -3390,13 +3384,13 @@
       <c r="P45" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="Q45" s="8">
+      <c r="Q45" s="1">
         <v>93</v>
       </c>
-      <c r="R45" s="11">
+      <c r="R45" s="9">
         <v>36650.4</v>
       </c>
-      <c r="S45" s="12">
+      <c r="S45" s="10">
         <v>37505.48</v>
       </c>
       <c r="T45" s="7" t="str">
@@ -3427,7 +3421,7 @@
       <c r="J46" s="5">
         <v>68</v>
       </c>
-      <c r="K46" s="11">
+      <c r="K46" s="9">
         <v>45462.43</v>
       </c>
       <c r="L46" s="6">
@@ -3440,13 +3434,13 @@
       <c r="P46" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="Q46" s="8">
+      <c r="Q46" s="1">
         <v>102</v>
       </c>
-      <c r="R46" s="11">
+      <c r="R46" s="9">
         <v>68368.27</v>
       </c>
-      <c r="S46" s="12">
+      <c r="S46" s="10">
         <v>72009.34</v>
       </c>
       <c r="T46" s="7" t="str">
@@ -3477,7 +3471,7 @@
       <c r="J47" s="5">
         <v>72</v>
       </c>
-      <c r="K47" s="11">
+      <c r="K47" s="9">
         <v>25880.31</v>
       </c>
       <c r="L47" s="6">
@@ -3490,13 +3484,13 @@
       <c r="P47" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Q47" s="8">
+      <c r="Q47" s="1">
         <v>108</v>
       </c>
-      <c r="R47" s="11">
+      <c r="R47" s="9">
         <v>40210.94</v>
       </c>
-      <c r="S47" s="12">
+      <c r="S47" s="10">
         <v>40210.94</v>
       </c>
       <c r="T47" s="7" t="str">
@@ -3527,7 +3521,7 @@
       <c r="J48" s="5">
         <v>76</v>
       </c>
-      <c r="K48" s="11">
+      <c r="K48" s="9">
         <v>32440.64</v>
       </c>
       <c r="L48" s="6">
@@ -3540,13 +3534,13 @@
       <c r="P48" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="Q48" s="8">
+      <c r="Q48" s="1">
         <v>114</v>
       </c>
-      <c r="R48" s="11">
+      <c r="R48" s="9">
         <v>46089.98</v>
       </c>
-      <c r="S48" s="12">
+      <c r="S48" s="10">
         <v>46089.98</v>
       </c>
       <c r="T48" s="7" t="str">
@@ -3577,7 +3571,7 @@
       <c r="J49" s="5">
         <v>113</v>
       </c>
-      <c r="K49" s="11">
+      <c r="K49" s="9">
         <v>41301.91</v>
       </c>
       <c r="L49" s="6">
@@ -3590,13 +3584,13 @@
       <c r="P49" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Q49" s="8">
+      <c r="Q49" s="1">
         <v>169</v>
       </c>
-      <c r="R49" s="11">
+      <c r="R49" s="9">
         <v>48188.7</v>
       </c>
-      <c r="S49" s="12">
+      <c r="S49" s="10">
         <v>48353.82</v>
       </c>
       <c r="T49" s="7" t="str">
@@ -3627,7 +3621,7 @@
       <c r="J50" s="5">
         <v>132</v>
       </c>
-      <c r="K50" s="11">
+      <c r="K50" s="9">
         <v>21568.72</v>
       </c>
       <c r="L50" s="6">
@@ -3640,13 +3634,13 @@
       <c r="P50" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Q50" s="8">
+      <c r="Q50" s="1">
         <v>198</v>
       </c>
-      <c r="R50" s="11">
+      <c r="R50" s="9">
         <v>33880.01</v>
       </c>
-      <c r="S50" s="12">
+      <c r="S50" s="10">
         <v>33977.04</v>
       </c>
       <c r="T50" s="7" t="str">
@@ -3677,7 +3671,7 @@
       <c r="J51" s="5">
         <v>149</v>
       </c>
-      <c r="K51" s="11">
+      <c r="K51" s="9">
         <v>23845.29</v>
       </c>
       <c r="L51" s="6">
@@ -3690,13 +3684,13 @@
       <c r="P51" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="Q51" s="8">
+      <c r="Q51" s="1">
         <v>224</v>
       </c>
-      <c r="R51" s="11">
+      <c r="R51" s="9">
         <v>34501.38</v>
       </c>
-      <c r="S51" s="12">
+      <c r="S51" s="10">
         <v>34504.73</v>
       </c>
       <c r="T51" s="7" t="str">
@@ -3727,7 +3721,7 @@
       <c r="J52" s="5">
         <v>219</v>
       </c>
-      <c r="K52" s="11">
+      <c r="K52" s="9">
         <v>36727.88</v>
       </c>
       <c r="L52" s="6">
@@ -3740,13 +3734,13 @@
       <c r="P52" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="Q52" s="8">
+      <c r="Q52" s="1">
         <v>329</v>
       </c>
-      <c r="R52" s="11">
+      <c r="R52" s="9">
         <v>61894.86</v>
       </c>
-      <c r="S52" s="12">
+      <c r="S52" s="10">
         <v>61894.86</v>
       </c>
       <c r="T52" s="7" t="str">
@@ -3777,7 +3771,7 @@
       <c r="J53" s="5">
         <v>501</v>
       </c>
-      <c r="K53" s="11">
+      <c r="K53" s="9">
         <v>117296.16</v>
       </c>
       <c r="L53" s="6">
@@ -3790,10 +3784,10 @@
       <c r="P53" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="Q53" s="8">
+      <c r="Q53" s="1">
         <v>751</v>
       </c>
-      <c r="R53" s="11">
+      <c r="R53" s="9">
         <v>184532.11</v>
       </c>
       <c r="S53" s="6" t="s">
@@ -3826,7 +3820,7 @@
       <c r="J54" s="5">
         <v>49</v>
       </c>
-      <c r="K54" s="11">
+      <c r="K54" s="9">
         <v>557.86</v>
       </c>
       <c r="L54" s="6">
@@ -3839,13 +3833,13 @@
       <c r="P54" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="Q54" s="8">
+      <c r="Q54" s="1">
         <v>74</v>
       </c>
-      <c r="R54" s="11">
+      <c r="R54" s="9">
         <v>864.95</v>
       </c>
-      <c r="S54" s="12">
+      <c r="S54" s="10">
         <v>856.88</v>
       </c>
       <c r="T54" s="7" t="str">
@@ -3876,7 +3870,7 @@
       <c r="J55" s="5">
         <v>97</v>
       </c>
-      <c r="K55" s="11">
+      <c r="K55" s="9">
         <v>1109.68</v>
       </c>
       <c r="L55" s="6">
@@ -3889,13 +3883,13 @@
       <c r="P55" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="Q55" s="8">
+      <c r="Q55" s="1">
         <v>146</v>
       </c>
-      <c r="R55" s="11">
+      <c r="R55" s="9">
         <v>1669.63</v>
       </c>
-      <c r="S55" s="12">
+      <c r="S55" s="10">
         <v>1669.63</v>
       </c>
       <c r="T55" s="7" t="str">
@@ -3926,7 +3920,7 @@
       <c r="J56" s="5">
         <v>287</v>
       </c>
-      <c r="K56" s="11">
+      <c r="K56" s="9">
         <v>3239.8</v>
       </c>
       <c r="L56" s="6">
@@ -3939,10 +3933,10 @@
       <c r="P56" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="Q56" s="8">
+      <c r="Q56" s="1">
         <v>431</v>
       </c>
-      <c r="R56" s="11">
+      <c r="R56" s="9">
         <v>5042.6</v>
       </c>
       <c r="S56" s="6" t="s">
@@ -3975,7 +3969,7 @@
       <c r="J57" s="5">
         <v>391</v>
       </c>
-      <c r="K57" s="11">
+      <c r="K57" s="9">
         <v>4281.01</v>
       </c>
       <c r="L57" s="6">
@@ -3988,10 +3982,10 @@
       <c r="P57" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Q57" s="8">
+      <c r="Q57" s="1">
         <v>587</v>
       </c>
-      <c r="R57" s="11">
+      <c r="R57" s="9">
         <v>6681.59</v>
       </c>
       <c r="S57" s="6" t="s">
@@ -4024,7 +4018,7 @@
       <c r="J58" s="5">
         <v>87</v>
       </c>
-      <c r="K58" s="11">
+      <c r="K58" s="9">
         <v>10179</v>
       </c>
       <c r="L58" s="6">
@@ -4037,13 +4031,13 @@
       <c r="P58" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="Q58" s="8">
+      <c r="Q58" s="1">
         <v>131</v>
       </c>
-      <c r="R58" s="11">
+      <c r="R58" s="9">
         <v>15733</v>
       </c>
-      <c r="S58" s="12">
+      <c r="S58" s="10">
         <v>15589</v>
       </c>
       <c r="T58" s="7" t="str">
@@ -4074,7 +4068,7 @@
       <c r="J59" s="5">
         <v>267</v>
       </c>
-      <c r="K59" s="11">
+      <c r="K59" s="9">
         <v>22763</v>
       </c>
       <c r="L59" s="6">
@@ -4087,10 +4081,10 @@
       <c r="P59" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Q59" s="8">
+      <c r="Q59" s="1">
         <v>401</v>
       </c>
-      <c r="R59" s="11">
+      <c r="R59" s="9">
         <v>35278</v>
       </c>
       <c r="S59" s="6" t="s">
@@ -4123,7 +4117,7 @@
       <c r="J60" s="5">
         <v>516</v>
       </c>
-      <c r="K60" s="11">
+      <c r="K60" s="9">
         <v>45504</v>
       </c>
       <c r="L60" s="6">
@@ -4136,10 +4130,10 @@
       <c r="P60" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Q60" s="8">
+      <c r="Q60" s="1">
         <v>774</v>
       </c>
-      <c r="R60" s="11">
+      <c r="R60" s="9">
         <v>69819</v>
       </c>
       <c r="S60" s="6" t="s">
@@ -4172,7 +4166,7 @@
       <c r="J61" s="5">
         <v>35</v>
       </c>
-      <c r="K61" s="11">
+      <c r="K61" s="9">
         <v>274.86</v>
       </c>
       <c r="L61" s="6">
@@ -4185,13 +4179,13 @@
       <c r="P61" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q61" s="8">
+      <c r="Q61" s="1">
         <v>52</v>
       </c>
-      <c r="R61" s="11">
+      <c r="R61" s="9">
         <v>440.64</v>
       </c>
-      <c r="S61" s="12">
+      <c r="S61" s="10">
         <v>440.07</v>
       </c>
       <c r="T61" s="7" t="str">
@@ -4222,7 +4216,7 @@
       <c r="J62" s="5">
         <v>21</v>
       </c>
-      <c r="K62" s="11">
+      <c r="K62" s="9">
         <v>425</v>
       </c>
       <c r="L62" s="6">
@@ -4235,13 +4229,13 @@
       <c r="P62" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="Q62" s="8">
+      <c r="Q62" s="1">
         <v>31</v>
       </c>
-      <c r="R62" s="11">
+      <c r="R62" s="9">
         <v>715</v>
       </c>
-      <c r="S62" s="12">
+      <c r="S62" s="10">
         <v>715</v>
       </c>
       <c r="T62" s="7" t="str">
@@ -4272,7 +4266,7 @@
       <c r="J63" s="5">
         <v>112</v>
       </c>
-      <c r="K63" s="11">
+      <c r="K63" s="9">
         <v>55500</v>
       </c>
       <c r="L63" s="6">
@@ -4285,13 +4279,13 @@
       <c r="P63" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="Q63" s="8">
+      <c r="Q63" s="1">
         <v>168</v>
       </c>
-      <c r="R63" s="11">
+      <c r="R63" s="9">
         <v>85571.07</v>
       </c>
-      <c r="S63" s="12">
+      <c r="S63" s="10">
         <v>85571.07</v>
       </c>
       <c r="T63" s="7" t="str">
@@ -4322,7 +4316,7 @@
       <c r="J64" s="5">
         <v>112</v>
       </c>
-      <c r="K64" s="11">
+      <c r="K64" s="9">
         <v>1760.09</v>
       </c>
       <c r="L64" s="6">
@@ -4335,13 +4329,13 @@
       <c r="P64" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Q64" s="8">
+      <c r="Q64" s="1">
         <v>168</v>
       </c>
-      <c r="R64" s="11">
+      <c r="R64" s="9">
         <v>2614.58</v>
       </c>
-      <c r="S64" s="12">
+      <c r="S64" s="10">
         <v>2654.69</v>
       </c>
       <c r="T64" s="7" t="str">
@@ -4372,7 +4366,7 @@
       <c r="J65" s="5">
         <v>8</v>
       </c>
-      <c r="K65" s="11">
+      <c r="K65" s="9">
         <v>1981.71</v>
       </c>
       <c r="L65" s="6">
@@ -4385,13 +4379,13 @@
       <c r="P65" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="Q65" s="8">
+      <c r="Q65" s="1">
         <v>12</v>
       </c>
-      <c r="R65" s="11">
+      <c r="R65" s="9">
         <v>2741.1</v>
       </c>
-      <c r="S65" s="12">
+      <c r="S65" s="10">
         <v>2741.1</v>
       </c>
       <c r="T65" s="7" t="str">
@@ -4422,7 +4416,7 @@
       <c r="J66" s="5">
         <v>11</v>
       </c>
-      <c r="K66" s="11">
+      <c r="K66" s="9">
         <v>2062.92</v>
       </c>
       <c r="L66" s="6">
@@ -4435,13 +4429,13 @@
       <c r="P66" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Q66" s="8">
+      <c r="Q66" s="1">
         <v>16</v>
       </c>
-      <c r="R66" s="11">
+      <c r="R66" s="9">
         <v>2540.07</v>
       </c>
-      <c r="S66" s="12">
+      <c r="S66" s="10">
         <v>2732.27</v>
       </c>
       <c r="T66" s="7" t="str">
@@ -4450,33 +4444,33 @@
       </c>
     </row>
     <row r="69" spans="2:4">
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
     </row>
     <row r="70" spans="2:4">
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C70" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D70" s="13" t="s">
+      <c r="D70" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="2:4">
-      <c r="B71" s="14">
+      <c r="B71" s="12">
         <f>COUNTIF(F5:F66,"RVND")+COUNTIF(M5:M66,"RVND")+COUNTIF(T5:T66,"RVND")</f>
         <v>41</v>
       </c>
-      <c r="C71" s="14">
+      <c r="C71" s="12">
         <f>COUNTIF(F5:F66,"ILS")+COUNTIF(M5:M66,"ILS")+COUNTIF(T5:T66,"ILS")</f>
         <v>38</v>
       </c>
-      <c r="D71" s="14">
+      <c r="D71" s="12">
         <f>COUNTIF(F5:F66,"Iguais")+COUNTIF(M5:M66,"Iguais")+COUNTIF(T5:T66,"Iguais")</f>
         <v>99</v>
       </c>

</xml_diff>